<commit_message>
#4 adding joker symbols - excel updated, reading joker symbols realized
</commit_message>
<xml_diff>
--- a/app/colony.xlsx
+++ b/app/colony.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="113">
   <si>
     <t>environment rows</t>
   </si>
@@ -343,6 +343,24 @@
   </si>
   <si>
     <t>animation delay, pause between displaying new iteration in seconds</t>
+  </si>
+  <si>
+    <t>JokerSymbolsBegin</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>a,b,c,d,f,p10,p9,p8,p7,p6,p5,p4,p3,p2,p1</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>JokerSymbolsEnd</t>
+  </si>
+  <si>
+    <t>p1,p2,p3,p4</t>
   </si>
 </sst>
 </file>
@@ -661,19 +679,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.140625" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -681,7 +700,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -689,7 +708,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -697,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>95</v>
       </c>
@@ -705,12 +724,38 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5">
         <v>0.91500000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#1 color settings in the excel - reading the settings from the excel and sending to the vizualization
</commit_message>
<xml_diff>
--- a/app/colony.xlsx
+++ b/app/colony.xlsx
@@ -17,12 +17,12 @@
     <sheet name="Environment_rules" sheetId="3" r:id="rId3"/>
     <sheet name="Agents" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="119">
   <si>
     <t>environment rows</t>
   </si>
@@ -361,6 +361,24 @@
   </si>
   <si>
     <t>p1,p2,p3,p4</t>
+  </si>
+  <si>
+    <t>ColorSettingsBegin</t>
+  </si>
+  <si>
+    <t>ColorSettingsEnd</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>green</t>
   </si>
 </sst>
 </file>
@@ -679,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,6 +774,32 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed error in function MarkInterest (visualize.py) - parameter colors is used now#1
</commit_message>
<xml_diff>
--- a/app/colony.xlsx
+++ b/app/colony.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valeodan\Desktop\develop\New\2dpcolony\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5F7A0-B56E-40C0-B76E-34C7184532F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13485"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -213,9 +214,6 @@
     <t>h,7</t>
   </si>
   <si>
-    <t>I,1</t>
-  </si>
-  <si>
     <t>I,2</t>
   </si>
   <si>
@@ -228,9 +226,6 @@
     <t>I,5</t>
   </si>
   <si>
-    <t>I,6</t>
-  </si>
-  <si>
     <t>I,7</t>
   </si>
   <si>
@@ -379,12 +374,18 @@
   </si>
   <si>
     <t>green</t>
+  </si>
+  <si>
+    <t>p,6</t>
+  </si>
+  <si>
+    <t>p,1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -696,21 +697,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.1796875" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,7 +719,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -726,7 +727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -734,72 +735,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B5">
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>108</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -808,16 +809,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -843,13 +844,13 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="J1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -875,13 +876,13 @@
         <v>57</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -907,13 +908,13 @@
         <v>58</v>
       </c>
       <c r="I3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -939,13 +940,13 @@
         <v>59</v>
       </c>
       <c r="I4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -971,13 +972,13 @@
         <v>60</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1003,13 +1004,13 @@
         <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1035,189 +1036,189 @@
         <v>62</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="8:20" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="N18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="R18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="T18" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="8:20" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H19" t="s">
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="R19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="T19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="8:20" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H20" t="s">
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="8:20" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H21" t="s">
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M21" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N21" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="8:20" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H22" t="s">
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N22" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="8:20" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H23" t="s">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="N24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1226,41 +1227,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1272,690 +1273,690 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G1">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I1">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K1">
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
         <v>79</v>
       </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
         <v>84</v>
-      </c>
-      <c r="D8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" t="s">
-        <v>80</v>
-      </c>
-      <c r="D15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F23" t="s">
-        <v>86</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="C25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" t="s">
+        <v>78</v>
+      </c>
+      <c r="D37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>75</v>
+      </c>
+      <c r="E38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="E42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
         <v>84</v>
-      </c>
-      <c r="D30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>79</v>
-      </c>
-      <c r="C33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C37" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" t="s">
-        <v>3</v>
-      </c>
-      <c r="D42" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45" t="s">
-        <v>103</v>
-      </c>
-      <c r="D45" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" t="s">
-        <v>93</v>
-      </c>
-      <c r="F45" t="s">
-        <v>86</v>
       </c>
       <c r="G45">
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I45">
         <v>3</v>
       </c>
       <c r="J45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" t="s">
         <v>79</v>
       </c>
-      <c r="C47" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" t="s">
+        <v>83</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B65" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" t="s">
-        <v>3</v>
-      </c>
-      <c r="D56" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C59" t="s">
-        <v>80</v>
-      </c>
-      <c r="D59" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>79</v>
-      </c>
-      <c r="C60" t="s">
-        <v>3</v>
-      </c>
-      <c r="D60" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>79</v>
-      </c>
-      <c r="C63" t="s">
-        <v>3</v>
-      </c>
-      <c r="D63" t="s">
-        <v>77</v>
-      </c>
-      <c r="E63" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>79</v>
-      </c>
-      <c r="C64" t="s">
-        <v>84</v>
-      </c>
-      <c r="D64" t="s">
-        <v>85</v>
-      </c>
-      <c r="E64" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4 joker symbols added for motion rules, bugfix for agent id when multiple copies entered, id of the agent sent into the object
</commit_message>
<xml_diff>
--- a/app/colony.xlsx
+++ b/app/colony.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valeodan\Desktop\develop\New\2dpcolony\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C5F7A0-B56E-40C0-B76E-34C7184532F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="120">
   <si>
     <t>environment rows</t>
   </si>
@@ -259,9 +258,6 @@
     <t>rule</t>
   </si>
   <si>
-    <t>e,e,e,e,e,e,e,e,e</t>
-  </si>
-  <si>
     <t>u</t>
   </si>
   <si>
@@ -331,9 +327,6 @@
     <t>Agent3</t>
   </si>
   <si>
-    <t>start I (-1 for random value)</t>
-  </si>
-  <si>
     <t>start j (-1 for random value)</t>
   </si>
   <si>
@@ -380,12 +373,21 @@
   </si>
   <si>
     <t>p,1</t>
+  </si>
+  <si>
+    <t>*,*,*,*,*,*,*,*,*</t>
+  </si>
+  <si>
+    <t>a,a,a,a,a,a,a,a,a</t>
+  </si>
+  <si>
+    <t>start i (-1 for random value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,21 +699,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.1796875" customWidth="1"/>
-    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -727,7 +729,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -735,72 +737,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5">
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>106</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>114</v>
-      </c>
-      <c r="C13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -809,16 +811,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -844,13 +846,13 @@
         <v>56</v>
       </c>
       <c r="I1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -882,7 +884,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -914,7 +916,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -946,7 +948,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -978,7 +980,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1004,13 +1006,13 @@
         <v>61</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1042,183 +1044,183 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="8:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="N18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="T18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="8:20" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="T19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="8:20" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="8:20" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="8:20" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N22" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="23" spans="8:20" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N23" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>3</v>
       </c>
       <c r="I24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1227,14 +1229,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1247,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1256,7 +1258,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1273,84 +1275,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
         <v>96</v>
-      </c>
-      <c r="C1" t="s">
-        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>76</v>
       </c>
       <c r="E1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="G1">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I1">
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K1">
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>77</v>
       </c>
       <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
         <v>78</v>
       </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" t="s">
         <v>75</v>
@@ -1359,33 +1361,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>77</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
         <v>75</v>
@@ -1394,33 +1396,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>77</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" t="s">
         <v>75</v>
@@ -1429,33 +1431,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>77</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>75</v>
@@ -1464,17 +1466,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>77</v>
       </c>
@@ -1485,88 +1487,88 @@
         <v>75</v>
       </c>
       <c r="E19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>88</v>
-      </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
         <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G23">
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I23">
         <v>3</v>
       </c>
       <c r="J23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>77</v>
       </c>
       <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
         <v>78</v>
       </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>77</v>
       </c>
@@ -1580,33 +1582,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
         <v>75</v>
@@ -1615,33 +1617,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" t="s">
         <v>75</v>
@@ -1650,52 +1652,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>77</v>
       </c>
       <c r="C37" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>77</v>
+      </c>
+      <c r="C38" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B38" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" t="s">
-        <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>77</v>
       </c>
@@ -1706,10 +1708,10 @@
         <v>75</v>
       </c>
       <c r="E41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>77</v>
       </c>
@@ -1723,71 +1725,71 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>88</v>
-      </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>76</v>
       </c>
       <c r="E45" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G45">
         <v>4</v>
       </c>
       <c r="H45" t="s">
+        <v>84</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45" t="s">
+        <v>97</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>85</v>
       </c>
-      <c r="I45">
-        <v>3</v>
-      </c>
-      <c r="J45" t="s">
-        <v>98</v>
-      </c>
-      <c r="K45">
-        <v>1</v>
-      </c>
-      <c r="L45" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>77</v>
       </c>
       <c r="C47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47" t="s">
         <v>78</v>
       </c>
-      <c r="D47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>77</v>
       </c>
@@ -1801,28 +1803,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>77</v>
       </c>
       <c r="C51" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>77</v>
       </c>
@@ -1836,28 +1838,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>77</v>
       </c>
       <c r="C55" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>77</v>
       </c>
@@ -1871,28 +1873,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>77</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="D59" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>77</v>
       </c>
@@ -1903,20 +1905,20 @@
         <v>75</v>
       </c>
       <c r="E60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>77</v>
       </c>
@@ -1927,36 +1929,36 @@
         <v>75</v>
       </c>
       <c r="E63" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="C64" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>77</v>
-      </c>
-      <c r="C64" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" t="s">
-        <v>83</v>
-      </c>
       <c r="E64" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed - sometimes the joker symbol is empty because the agent is on the border of the environment. This caused the crashes of the app. Empty joker symbol is currently replaced by "e".
</commit_message>
<xml_diff>
--- a/app/colony.xlsx
+++ b/app/colony.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\personal\vsb\projekty\aco_simulator\2dpcolony\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valeodan\Desktop\develop\New\2dpcolony\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5128DEA5-CC1C-418A-BEFE-FC988C10208F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305" activeTab="3"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="118">
   <si>
     <t>environment rows</t>
   </si>
@@ -159,9 +160,6 @@
     <t>f,3</t>
   </si>
   <si>
-    <t>f,4</t>
-  </si>
-  <si>
     <t>f,5</t>
   </si>
   <si>
@@ -258,6 +256,9 @@
     <t>rule</t>
   </si>
   <si>
+    <t>e,e,e,e,e,e,e,e,e</t>
+  </si>
+  <si>
     <t>u</t>
   </si>
   <si>
@@ -327,6 +328,9 @@
     <t>Agent3</t>
   </si>
   <si>
+    <t>start I (-1 for random value)</t>
+  </si>
+  <si>
     <t>start j (-1 for random value)</t>
   </si>
   <si>
@@ -357,9 +361,6 @@
     <t>ColorSettingsEnd</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -375,19 +376,13 @@
     <t>p,1</t>
   </si>
   <si>
-    <t>*,*,*,*,*,*,*,*,*</t>
-  </si>
-  <si>
-    <t>a,a,a,a,a,a,a,a,a</t>
-  </si>
-  <si>
-    <t>start i (-1 for random value)</t>
+    <t>p,4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -699,21 +694,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="142.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="142.1796875" customWidth="1"/>
+    <col min="7" max="7" width="20.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -721,7 +716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -729,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -737,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -745,54 +740,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B5">
         <v>0.91500000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>112</v>
       </c>
@@ -800,9 +795,9 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -811,16 +806,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -840,19 +835,19 @@
         <v>42</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I1" t="s">
         <v>116</v>
       </c>
       <c r="J1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -872,19 +867,19 @@
         <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -904,19 +899,19 @@
         <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -933,22 +928,22 @@
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="G4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -965,22 +960,22 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -997,22 +992,22 @@
         <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" t="s">
         <v>115</v>
       </c>
       <c r="J6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1029,22 +1024,22 @@
         <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="8:20" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H18" t="s">
         <v>94</v>
       </c>
@@ -1076,7 +1071,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H19" t="s">
         <v>3</v>
       </c>
@@ -1108,7 +1103,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H20" t="s">
         <v>3</v>
       </c>
@@ -1131,7 +1126,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H21" t="s">
         <v>3</v>
       </c>
@@ -1154,7 +1149,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H22" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1172,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H23" t="s">
         <v>3</v>
       </c>
@@ -1200,7 +1195,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="24" spans="8:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:20" x14ac:dyDescent="0.35">
       <c r="H24" t="s">
         <v>3</v>
       </c>
@@ -1229,41 +1224,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -1275,25 +1270,25 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="80.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="80.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -1304,19 +1299,19 @@
         <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
         <v>90</v>
       </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="G1">
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I1">
         <v>3</v>
@@ -1331,168 +1326,168 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
         <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>117</v>
       </c>
       <c r="D3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>81</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
         <v>77</v>
-      </c>
-      <c r="C7" t="s">
-        <v>117</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
         <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
         <v>77</v>
-      </c>
-      <c r="C11" t="s">
-        <v>117</v>
       </c>
       <c r="D11" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
         <v>81</v>
       </c>
       <c r="D12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
-      </c>
-      <c r="C15" t="s">
-        <v>117</v>
       </c>
       <c r="D15" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
         <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
         <v>91</v>
@@ -1504,17 +1499,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1525,7 +1520,7 @@
         <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
         <v>90</v>
@@ -1552,190 +1547,190 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
       </c>
       <c r="D25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E26" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
         <v>77</v>
-      </c>
-      <c r="C29" t="s">
-        <v>118</v>
       </c>
       <c r="D29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
         <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E30" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" t="s">
         <v>77</v>
-      </c>
-      <c r="C33" t="s">
-        <v>118</v>
       </c>
       <c r="D33" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
         <v>81</v>
       </c>
       <c r="D34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E34" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
         <v>77</v>
-      </c>
-      <c r="C37" t="s">
-        <v>118</v>
       </c>
       <c r="D37" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
         <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41" t="s">
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E41" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>87</v>
       </c>
@@ -1746,7 +1741,7 @@
         <v>100</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
         <v>90</v>
@@ -1767,174 +1762,174 @@
         <v>97</v>
       </c>
       <c r="K45">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" t="s">
         <v>77</v>
-      </c>
-      <c r="C47" t="s">
-        <v>118</v>
       </c>
       <c r="D47" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" t="s">
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" t="s">
         <v>77</v>
-      </c>
-      <c r="C51" t="s">
-        <v>118</v>
       </c>
       <c r="D51" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" t="s">
         <v>77</v>
-      </c>
-      <c r="C55" t="s">
-        <v>118</v>
       </c>
       <c r="D55" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E56" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" t="s">
         <v>77</v>
-      </c>
-      <c r="C59" t="s">
-        <v>118</v>
       </c>
       <c r="D59" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E60" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E63" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" t="s">
         <v>81</v>
@@ -1946,17 +1941,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>89</v>
       </c>

</xml_diff>